<commit_message>
tpo in effect size table
</commit_message>
<xml_diff>
--- a/docs/source/concept_models/vivarium_gates_bep/child_growth_birthweight_correlations.xlsx
+++ b/docs/source/concept_models/vivarium_gates_bep/child_growth_birthweight_correlations.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vivarium_research\docs\source\gbd2017_models\concept_models\vivarium_gates_bep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vivarium_research\docs\source\concept_models\vivarium_gates_bep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="19155" windowHeight="6360"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20355" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="child_growth_birthweight_correl" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -587,6 +588,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>151530</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="504825" y="790575"/>
+          <a:ext cx="6961905" cy="800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -854,14 +898,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2109,4 +2155,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>